<commit_message>
exo maison + change folder
</commit_message>
<xml_diff>
--- a/7 - Traitement de données en tables/Projet Traitement de données en tables/project/site/Magasins Angers.xlsx
+++ b/7 - Traitement de données en tables/Projet Traitement de données en tables/project/site/Magasins Angers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeweenH\PycharmProjects\NSI\7 - Traitement de données en tables\Projet Traitement de données en tables\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LeweenH\PycharmProjects\NSI\7 - Traitement de données en tables\Projet Traitement de données en tables\project\site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DBDF51-59FD-4349-AD2D-2F3858129F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A080F6-60E6-4184-BEB6-97A876CF884D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Maine et Loire</t>
   </si>
   <si>
-    <t>Carrefour Saiunt Serge</t>
-  </si>
-  <si>
     <t>Carrefour Grand Maine</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Carrefour Saint Serge</t>
   </si>
 </sst>
 </file>
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,228 +551,228 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
         <v>40</v>
       </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
         <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>